<commit_message>
Primeiro teste de filas deu certo
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="49">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -1461,10 +1461,14 @@
         <v>28</v>
       </c>
       <c r="B37" s="9">
+        <v>43608</v>
+      </c>
+      <c r="C37" s="9">
+        <v>43609</v>
+      </c>
+      <c r="D37" s="9">
         <v>43610</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
@@ -1827,15 +1831,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.28515625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="29" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -1907,181 +1910,301 @@
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B5" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="B6" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
+      <c r="B8" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="1">
+        <v>43576</v>
+      </c>
+      <c r="C10" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="B12" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="B14" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="B16" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B17" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
+      <c r="B19" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="1">
-        <v>43580</v>
-      </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B21" s="1">
+        <v>43587</v>
+      </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
+      <c r="B22" s="1">
+        <v>43539</v>
+      </c>
+      <c r="C22" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="B23" s="1">
+        <v>43569</v>
+      </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="B24" s="1">
+        <v>43549</v>
+      </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="B25" s="1">
+        <v>43568</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="B26" s="1">
+        <v>43562</v>
+      </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="B27" s="1">
+        <v>43568</v>
+      </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="B28" s="1">
+        <v>43561</v>
+      </c>
+      <c r="C28" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="B30" s="1">
+        <v>43587</v>
+      </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="B31" s="1">
+        <v>43539</v>
+      </c>
+      <c r="C31" s="1">
+        <v>43576</v>
+      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
+      <c r="B32" s="1">
+        <v>43569</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
+      <c r="B33" s="1">
+        <v>43549</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
+      <c r="B34" s="1">
+        <v>43568</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:2">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
+      <c r="B36" s="1">
+        <v>43549</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="B37" s="1">
+        <v>43568</v>
       </c>
     </row>
   </sheetData>
@@ -2490,8 +2613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2792,6 +2915,9 @@
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
+      <c r="B32" s="1">
+        <v>43549</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">

</xml_diff>

<commit_message>
incluido antiguidades para fila roxa
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -144,15 +144,6 @@
   </si>
   <si>
     <t>VERMELHA</t>
-  </si>
-  <si>
-    <t>TESTE1</t>
-  </si>
-  <si>
-    <t>TESTE2</t>
-  </si>
-  <si>
-    <t>TESTE3</t>
   </si>
   <si>
     <t>PRETA</t>
@@ -685,7 +676,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -758,987 +749,978 @@
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="19">
         <v>43611</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="19">
         <v>43612</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="19">
         <v>43613</v>
       </c>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="19"/>
+      <c r="P8" s="19"/>
+      <c r="Q8" s="19"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="P9" s="9"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="19"/>
+      <c r="P9" s="19"/>
+      <c r="Q9" s="19"/>
+      <c r="R9" s="19"/>
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="P10" s="9"/>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-      <c r="T10" s="9"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="19"/>
+      <c r="Q10" s="19"/>
+      <c r="R10" s="19"/>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19"/>
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
+      <c r="O12" s="19"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="19"/>
+      <c r="P13" s="19"/>
+      <c r="Q13" s="19"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
     </row>
     <row r="15" spans="1:20">
       <c r="A15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-      <c r="T15" s="9"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
     </row>
     <row r="16" spans="1:20">
       <c r="A16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-      <c r="T16" s="9"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="19"/>
+      <c r="P16" s="19"/>
+      <c r="Q16" s="19"/>
+      <c r="R16" s="19"/>
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
     </row>
     <row r="17" spans="1:20">
       <c r="A17" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
     </row>
     <row r="18" spans="1:20">
       <c r="A18" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
     </row>
     <row r="19" spans="1:20">
       <c r="A19" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
+      <c r="M19" s="19"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="19"/>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+      <c r="R19" s="19"/>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
     </row>
     <row r="20" spans="1:20">
       <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
-      <c r="Q21" s="9"/>
-      <c r="R21" s="9"/>
-      <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="19"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="19"/>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+      <c r="R21" s="19"/>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="9"/>
-      <c r="T22" s="9"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+      <c r="R22" s="19"/>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
-      <c r="Q23" s="9"/>
-      <c r="R23" s="9"/>
-      <c r="S23" s="9"/>
-      <c r="T23" s="9"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
     </row>
     <row r="24" spans="1:20">
       <c r="A24" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="9"/>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-      <c r="M24" s="9"/>
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="9"/>
-      <c r="Q24" s="9"/>
-      <c r="R24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="T24" s="9"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="9"/>
-      <c r="N25" s="9"/>
-      <c r="O25" s="9"/>
-      <c r="P25" s="9"/>
-      <c r="Q25" s="9"/>
-      <c r="R25" s="9"/>
-      <c r="S25" s="9"/>
-      <c r="T25" s="9"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="19"/>
+      <c r="Q25" s="19"/>
+      <c r="R25" s="19"/>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
     </row>
     <row r="26" spans="1:20">
       <c r="A26" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-      <c r="M26" s="9"/>
-      <c r="N26" s="9"/>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9"/>
-      <c r="Q26" s="9"/>
-      <c r="R26" s="9"/>
-      <c r="S26" s="9"/>
-      <c r="T26" s="9"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="9"/>
-      <c r="N28" s="9"/>
-      <c r="O28" s="9"/>
-      <c r="P28" s="9"/>
-      <c r="Q28" s="9"/>
-      <c r="R28" s="9"/>
-      <c r="S28" s="9"/>
-      <c r="T28" s="9"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
     </row>
     <row r="29" spans="1:20">
       <c r="A29" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-      <c r="M29" s="9"/>
-      <c r="N29" s="9"/>
-      <c r="O29" s="9"/>
-      <c r="P29" s="9"/>
-      <c r="Q29" s="9"/>
-      <c r="R29" s="9"/>
-      <c r="S29" s="9"/>
-      <c r="T29" s="9"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-      <c r="M30" s="9"/>
-      <c r="N30" s="9"/>
-      <c r="O30" s="9"/>
-      <c r="P30" s="9"/>
-      <c r="Q30" s="9"/>
-      <c r="R30" s="9"/>
-      <c r="S30" s="9"/>
-      <c r="T30" s="9"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
     </row>
     <row r="31" spans="1:20">
       <c r="A31" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-      <c r="M31" s="9"/>
-      <c r="N31" s="9"/>
-      <c r="O31" s="9"/>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
-      <c r="S31" s="9"/>
-      <c r="T31" s="9"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
     </row>
     <row r="32" spans="1:20">
       <c r="A32" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="9"/>
-      <c r="P32" s="9"/>
-      <c r="Q32" s="9"/>
-      <c r="R32" s="9"/>
-      <c r="S32" s="9"/>
-      <c r="T32" s="9"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
     </row>
     <row r="33" spans="1:20">
       <c r="A33" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-      <c r="M33" s="9"/>
-      <c r="N33" s="9"/>
-      <c r="O33" s="9"/>
-      <c r="P33" s="9"/>
-      <c r="Q33" s="9"/>
-      <c r="R33" s="9"/>
-      <c r="S33" s="9"/>
-      <c r="T33" s="9"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
-      <c r="J34" s="9"/>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
-      <c r="M34" s="9"/>
-      <c r="N34" s="9"/>
-      <c r="O34" s="9"/>
-      <c r="P34" s="9"/>
-      <c r="Q34" s="9"/>
-      <c r="R34" s="9"/>
-      <c r="S34" s="9"/>
-      <c r="T34" s="9"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
     </row>
     <row r="35" spans="1:20">
       <c r="A35" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="9"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="9"/>
-      <c r="P35" s="9"/>
-      <c r="Q35" s="9"/>
-      <c r="R35" s="9"/>
-      <c r="S35" s="9"/>
-      <c r="T35" s="9"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
     </row>
     <row r="36" spans="1:20">
       <c r="A36" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9"/>
-      <c r="Q36" s="9"/>
-      <c r="R36" s="9"/>
-      <c r="S36" s="9"/>
-      <c r="T36" s="9"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
     </row>
     <row r="37" spans="1:20">
       <c r="A37" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="9">
+      <c r="B37" s="19">
         <v>43608</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="19">
         <v>43609</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="19">
         <v>43610</v>
       </c>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="9"/>
-      <c r="P37" s="9"/>
-      <c r="Q37" s="9"/>
-      <c r="R37" s="9"/>
-      <c r="S37" s="9"/>
-      <c r="T37" s="9"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
     </row>
     <row r="38" spans="1:20">
       <c r="A38" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="9"/>
-      <c r="P38" s="9"/>
-      <c r="Q38" s="9"/>
-      <c r="R38" s="9"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="9"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
     </row>
     <row r="39" spans="1:20">
       <c r="A39" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="9">
+      <c r="B39" s="19">
         <v>43590</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="19">
         <v>43600</v>
       </c>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="K39" s="9"/>
-      <c r="L39" s="9"/>
-      <c r="M39" s="9"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
-      <c r="Q39" s="9"/>
-      <c r="R39" s="9"/>
-      <c r="S39" s="9"/>
-      <c r="T39" s="9"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
     </row>
     <row r="40" spans="1:20">
       <c r="A40" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="9">
+      <c r="B40" s="19">
         <v>43593</v>
       </c>
-      <c r="C40" s="9">
-        <v>43608</v>
-      </c>
-      <c r="D40" s="9">
+      <c r="C40" s="19">
         <v>43609</v>
       </c>
-      <c r="E40" s="9">
+      <c r="D40" s="19">
         <v>43610</v>
       </c>
-      <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
-      <c r="J40" s="9"/>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
-      <c r="M40" s="9"/>
-      <c r="N40" s="9"/>
-      <c r="O40" s="9"/>
-      <c r="P40" s="9"/>
-      <c r="Q40" s="9"/>
-      <c r="R40" s="9"/>
-      <c r="S40" s="9"/>
-      <c r="T40" s="9"/>
+      <c r="E40" s="19">
+        <v>43611</v>
+      </c>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="9">
+      <c r="B41" s="19">
         <v>43590</v>
       </c>
-      <c r="C41" s="9">
+      <c r="C41" s="19">
         <v>43591</v>
       </c>
-      <c r="D41" s="9">
+      <c r="D41" s="19">
         <v>43592</v>
       </c>
-      <c r="E41" s="9">
+      <c r="E41" s="19">
         <v>43593</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9"/>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
-      <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9"/>
-      <c r="Q41" s="9"/>
-      <c r="R41" s="9"/>
-      <c r="S41" s="9"/>
-      <c r="T41" s="9"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="19"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
+      <c r="L41" s="19"/>
+      <c r="M41" s="19"/>
+      <c r="N41" s="19"/>
+      <c r="O41" s="19"/>
+      <c r="P41" s="19"/>
+      <c r="Q41" s="19"/>
+      <c r="R41" s="19"/>
+      <c r="S41" s="19"/>
+      <c r="T41" s="19"/>
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
-      <c r="J42" s="9"/>
-      <c r="K42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
-      <c r="N42" s="9"/>
-      <c r="O42" s="9"/>
-      <c r="P42" s="9"/>
-      <c r="Q42" s="9"/>
-      <c r="R42" s="9"/>
-      <c r="S42" s="9"/>
-      <c r="T42" s="9"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="19"/>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="19"/>
+      <c r="M42" s="19"/>
+      <c r="N42" s="19"/>
+      <c r="O42" s="19"/>
+      <c r="P42" s="19"/>
+      <c r="Q42" s="19"/>
+      <c r="R42" s="19"/>
+      <c r="S42" s="19"/>
+      <c r="T42" s="19"/>
     </row>
     <row r="43" spans="1:20">
-      <c r="A43" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
-      <c r="J43" s="9"/>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
-      <c r="M43" s="9"/>
-      <c r="N43" s="9"/>
-      <c r="O43" s="9"/>
-      <c r="P43" s="9"/>
-      <c r="Q43" s="9"/>
-      <c r="R43" s="9"/>
-      <c r="S43" s="9"/>
-      <c r="T43" s="9"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19"/>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19"/>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19"/>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="19"/>
+      <c r="S43" s="19"/>
+      <c r="T43" s="19"/>
     </row>
     <row r="44" spans="1:20">
-      <c r="A44" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
+      <c r="L44" s="19"/>
+      <c r="M44" s="19"/>
+      <c r="N44" s="19"/>
+      <c r="O44" s="19"/>
+      <c r="P44" s="19"/>
+      <c r="Q44" s="19"/>
+      <c r="R44" s="19"/>
+      <c r="S44" s="19"/>
+      <c r="T44" s="19"/>
     </row>
     <row r="45" spans="1:20">
-      <c r="A45" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="9"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
-      <c r="J45" s="9"/>
-      <c r="K45" s="9"/>
-      <c r="L45" s="9"/>
-      <c r="M45" s="9"/>
-      <c r="N45" s="9"/>
-      <c r="O45" s="9"/>
-      <c r="P45" s="9"/>
-      <c r="Q45" s="9"/>
-      <c r="R45" s="9"/>
-      <c r="S45" s="9"/>
-      <c r="T45" s="9"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="19"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="19"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
+      <c r="J45" s="19"/>
+      <c r="K45" s="19"/>
+      <c r="L45" s="19"/>
+      <c r="M45" s="19"/>
+      <c r="N45" s="19"/>
+      <c r="O45" s="19"/>
+      <c r="P45" s="19"/>
+      <c r="Q45" s="19"/>
+      <c r="R45" s="19"/>
+      <c r="S45" s="19"/>
+      <c r="T45" s="19"/>
     </row>
     <row r="46" spans="1:20">
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="9"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="19"/>
+      <c r="H46" s="19"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="19"/>
+      <c r="K46" s="19"/>
+      <c r="L46" s="19"/>
+      <c r="M46" s="19"/>
+      <c r="N46" s="19"/>
+      <c r="O46" s="19"/>
+      <c r="P46" s="19"/>
+      <c r="Q46" s="19"/>
+      <c r="R46" s="19"/>
+      <c r="S46" s="19"/>
+      <c r="T46" s="19"/>
     </row>
     <row r="47" spans="1:20">
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="9"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9"/>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="9"/>
-      <c r="N47" s="9"/>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9"/>
-      <c r="Q47" s="9"/>
-      <c r="R47" s="9"/>
-      <c r="S47" s="9"/>
-      <c r="T47" s="9"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
     </row>
     <row r="48" spans="1:20">
       <c r="B48" s="9"/>
@@ -1925,7 +1907,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1">
         <v>43576</v>
@@ -1952,7 +1934,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -1968,7 +1950,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1">
         <v>43576</v>
@@ -1990,7 +1972,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1">
         <v>43576</v>
@@ -2009,7 +1991,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:29">
@@ -2025,7 +2007,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1">
         <v>43576</v>
@@ -2052,7 +2034,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2143,7 +2125,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1">
         <v>43576</v>
@@ -2235,7 +2217,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="29" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -2403,7 +2385,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2416,7 +2398,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +2424,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -2615,7 +2597,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2632,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2646,7 +2628,7 @@
   <sheetData>
     <row r="1" spans="1:29" s="25" customFormat="1" ht="26.25">
       <c r="A1" s="30" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -2682,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1">
         <v>43459</v>
@@ -2693,7 +2675,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -2717,7 +2699,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -2733,7 +2715,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1">
         <v>43576</v>
@@ -2744,7 +2726,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -2760,7 +2742,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1">
         <v>43576</v>
@@ -2787,7 +2769,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:29">
@@ -2803,7 +2785,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1">
         <v>43576</v>
@@ -2825,7 +2807,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1">
         <v>43576</v>
@@ -2844,7 +2826,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2860,7 +2842,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1">
         <v>43576</v>
@@ -2887,7 +2869,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2929,9 +2911,6 @@
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1">
-        <v>43569</v>
-      </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
@@ -2978,7 +2957,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C37" s="1">
         <v>43576</v>

</xml_diff>

<commit_message>
quase tirando da 24h
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -1481,8 +1481,12 @@
       <c r="A38" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
+      <c r="B38" s="19">
+        <v>43611</v>
+      </c>
+      <c r="C38" s="19">
+        <v>43610</v>
+      </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -2614,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
criação do arquivo escala.py
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -675,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -1460,7 +1460,9 @@
       <c r="D37" s="19">
         <v>43610</v>
       </c>
-      <c r="E37" s="19"/>
+      <c r="E37" s="19">
+        <v>43611</v>
+      </c>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
@@ -1484,9 +1486,7 @@
       <c r="B38" s="19">
         <v>43611</v>
       </c>
-      <c r="C38" s="19">
-        <v>43610</v>
-      </c>
+      <c r="C38" s="19"/>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -2618,9 +2618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>

<commit_message>
Refatorando colocando lastro como dicionario
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="46">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -675,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
   <cols>
@@ -713,10 +713,10 @@
         <v>36</v>
       </c>
       <c r="B4" s="19">
-        <v>43593</v>
+        <v>43617</v>
       </c>
       <c r="C4" s="19">
-        <v>43596</v>
+        <v>43619</v>
       </c>
       <c r="D4" s="19"/>
     </row>
@@ -747,15 +747,9 @@
       <c r="A8" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="19">
-        <v>43611</v>
-      </c>
-      <c r="C8" s="19">
-        <v>43612</v>
-      </c>
-      <c r="D8" s="19">
-        <v>43613</v>
-      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
       <c r="E8" s="19"/>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
@@ -801,7 +795,9 @@
       <c r="A10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="19"/>
+      <c r="B10" s="19">
+        <v>43617</v>
+      </c>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1821,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1901,27 +1897,21 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>43576</v>
+        <v>43556</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43576</v>
+      <c r="B4" s="1">
+        <v>43557</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
@@ -2190,9 +2180,6 @@
     <row r="36" spans="1:2">
       <c r="A36" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="B36" s="1">
-        <v>43549</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2213,7 +2200,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2428,7 +2415,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -2635,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2789,9 +2776,6 @@
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="5" t="s">

</xml_diff>

<commit_message>
escala vermelha (Falta resolver intervalo 24h)
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -675,7 +675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView topLeftCell="A7" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
   <cols>
@@ -1818,7 +1818,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1896,8 +1896,8 @@
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>43556</v>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:29">
@@ -1912,6 +1912,9 @@
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
@@ -2181,13 +2184,13 @@
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B37" s="1">
-        <v>43568</v>
       </c>
     </row>
   </sheetData>
@@ -2199,8 +2202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2211,77 +2214,80 @@
     <col min="30" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25">
+    <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="29" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" s="1">
+        <v>43454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -2415,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2427,77 +2433,80 @@
     <col min="30" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25">
+    <row r="1" spans="1:2" ht="26.25">
       <c r="A1" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
+      <c r="B3" s="1">
+        <v>43325</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -2623,7 +2632,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2671,8 +2680,8 @@
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
+      <c r="B3" s="1">
+        <v>42725</v>
       </c>
       <c r="C3" s="1">
         <v>43459</v>

</xml_diff>

<commit_message>
Tudo ok, (falta organizar a ordem da escala, iniciar por roxa, marrom, vermelha, preta.
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -675,7 +675,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
   <cols>
@@ -699,25 +701,21 @@
         <v>35</v>
       </c>
       <c r="B3" s="17">
-        <v>43640</v>
+        <v>43641</v>
       </c>
       <c r="C3" s="17">
-        <v>43641</v>
-      </c>
-      <c r="D3" s="17">
         <v>43642</v>
       </c>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="1:20" s="20" customFormat="1" ht="15.75">
       <c r="A4" s="12" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="19">
-        <v>43617</v>
-      </c>
-      <c r="C4" s="19">
-        <v>43619</v>
-      </c>
+        <v>43621</v>
+      </c>
+      <c r="C4" s="19"/>
       <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:20" s="22" customFormat="1">
@@ -1229,7 +1227,9 @@
       <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="19"/>
+      <c r="B28" s="19">
+        <v>43643</v>
+      </c>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
@@ -1480,7 +1480,9 @@
       <c r="B38" s="19">
         <v>43611</v>
       </c>
-      <c r="C38" s="19"/>
+      <c r="C38" s="19">
+        <v>43619</v>
+      </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -1595,7 +1597,9 @@
       <c r="A42" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="19"/>
+      <c r="B42" s="19">
+        <v>43618</v>
+      </c>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
@@ -1817,7 +1821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -2202,8 +2206,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2421,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2511,85 +2515,82 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1">
-        <v>43630</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
@@ -2607,6 +2608,9 @@
     <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43630</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2631,8 +2635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2906,9 +2910,6 @@
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="1">
-        <v>43640</v>
-      </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">

</xml_diff>

<commit_message>
Parece Tudo ok (Falta bateria de testes
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="3"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="45">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>MARROM</t>
-  </si>
-  <si>
-    <t>Lastro</t>
   </si>
 </sst>
 </file>
@@ -675,9 +672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
   <cols>
@@ -793,9 +788,7 @@
       <c r="A10" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="19">
-        <v>43617</v>
-      </c>
+      <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1227,9 +1220,7 @@
       <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="19">
-        <v>43643</v>
-      </c>
+      <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
       <c r="E28" s="19"/>
@@ -1325,7 +1316,9 @@
       <c r="A32" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="19"/>
+      <c r="B32" s="19">
+        <v>43645</v>
+      </c>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
       <c r="E32" s="19"/>
@@ -1445,18 +1438,10 @@
       <c r="A37" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B37" s="19">
-        <v>43608</v>
-      </c>
-      <c r="C37" s="19">
-        <v>43609</v>
-      </c>
-      <c r="D37" s="19">
-        <v>43610</v>
-      </c>
-      <c r="E37" s="19">
-        <v>43611</v>
-      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
       <c r="F37" s="19"/>
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
@@ -1478,11 +1463,9 @@
         <v>29</v>
       </c>
       <c r="B38" s="19">
-        <v>43611</v>
-      </c>
-      <c r="C38" s="19">
-        <v>43619</v>
-      </c>
+        <v>43644</v>
+      </c>
+      <c r="C38" s="19"/>
       <c r="D38" s="19"/>
       <c r="E38" s="19"/>
       <c r="F38" s="19"/>
@@ -1505,12 +1488,8 @@
       <c r="A39" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="19">
-        <v>43590</v>
-      </c>
-      <c r="C39" s="19">
-        <v>43600</v>
-      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="19"/>
       <c r="E39" s="19"/>
       <c r="F39" s="19"/>
@@ -1533,18 +1512,10 @@
       <c r="A40" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="19">
-        <v>43593</v>
-      </c>
-      <c r="C40" s="19">
-        <v>43609</v>
-      </c>
-      <c r="D40" s="19">
-        <v>43610</v>
-      </c>
-      <c r="E40" s="19">
-        <v>43611</v>
-      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
       <c r="F40" s="19"/>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
@@ -1565,18 +1536,10 @@
       <c r="A41" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="19">
-        <v>43590</v>
-      </c>
-      <c r="C41" s="19">
-        <v>43591</v>
-      </c>
-      <c r="D41" s="19">
-        <v>43592</v>
-      </c>
-      <c r="E41" s="19">
-        <v>43593</v>
-      </c>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
       <c r="F41" s="19"/>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
@@ -1597,9 +1560,7 @@
       <c r="A42" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="19">
-        <v>43618</v>
-      </c>
+      <c r="B42" s="19"/>
       <c r="C42" s="19"/>
       <c r="D42" s="19"/>
       <c r="E42" s="19"/>
@@ -1821,8 +1782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1900,299 +1861,173 @@
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>43557</v>
-      </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1">
-        <v>43576</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1">
-        <v>43600</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1">
-        <v>43607</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1">
-        <v>43539</v>
-      </c>
-      <c r="C22" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1">
-        <v>43569</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="1">
-        <v>43549</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1">
-        <v>43562</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+    </row>
+    <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="1">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    </row>
+    <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="1">
-        <v>43561</v>
-      </c>
-      <c r="C28" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+    </row>
+    <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+    </row>
+    <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="1">
-        <v>43624</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1">
-        <v>43539</v>
-      </c>
-      <c r="C31" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="1">
-        <v>43569</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="1">
-        <v>43549</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+    </row>
+    <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1">
-        <v>43617</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
@@ -2207,7 +2042,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B37" sqref="B29:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2296,124 +2131,109 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="1">
-        <v>43604</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+    </row>
+    <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="1">
-        <v>43604</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+    </row>
+    <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1">
-        <v>43627</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+    </row>
+    <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2425,8 +2245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2437,80 +2257,77 @@
     <col min="30" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25">
+    <row r="1" spans="1:1" ht="26.25">
       <c r="A1" s="31" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>43325</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+    </row>
+    <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:1">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:1">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:1">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:1">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:1">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:1">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -2595,33 +2412,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="1">
-        <v>43630</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+    </row>
+    <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+    </row>
+    <row r="37" spans="1:1">
       <c r="A37" s="4" t="s">
         <v>33</v>
       </c>
@@ -2635,8 +2446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2684,106 +2495,61 @@
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
-        <v>42725</v>
-      </c>
-      <c r="C3" s="1">
-        <v>43459</v>
-      </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="1">
-        <v>43576</v>
-      </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="5" t="s">
@@ -2794,203 +2560,116 @@
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+    </row>
+    <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1">
-        <v>43576</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+    </row>
+    <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+    </row>
+    <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C23" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+    </row>
+    <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+    </row>
+    <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+    </row>
+    <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+    </row>
+    <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+    </row>
+    <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="1">
-        <v>43529</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+    </row>
+    <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="1">
-        <v>43539</v>
-      </c>
-      <c r="C30" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+    </row>
+    <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="1">
-        <v>43609</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+    </row>
+    <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="1">
-        <v>43549</v>
-      </c>
-      <c r="C32" s="1">
-        <v>43642</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B33" s="1">
-        <v>43568</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>43641</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="1">
-        <v>43610</v>
-      </c>
-      <c r="C34" s="1">
-        <v>43641</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B35" s="1">
-        <v>43568</v>
-      </c>
-      <c r="C35" s="1">
-        <v>43611</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>43642</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="1">
-        <v>43561</v>
-      </c>
-      <c r="C36" s="1">
-        <v>43576</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" s="1">
-        <v>43576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tudo Ok exportando para o excel (Falta formatação)
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Preta" sheetId="4" r:id="rId3"/>
     <sheet name="Marrom" sheetId="5" r:id="rId4"/>
     <sheet name="Roxa" sheetId="6" r:id="rId5"/>
+    <sheet name="Escala" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -672,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -1791,7 +1792,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2053,7 +2054,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B37" sqref="B29:B37"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2256,7 +2257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -2686,4 +2687,16 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tudo Ok (Falta fazer escala reserva)
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,13 @@
     <sheet name="Preta" sheetId="4" r:id="rId3"/>
     <sheet name="Marrom" sheetId="5" r:id="rId4"/>
     <sheet name="Roxa" sheetId="6" r:id="rId5"/>
-    <sheet name="Escala" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="48">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -154,6 +153,15 @@
   </si>
   <si>
     <t>MARROM</t>
+  </si>
+  <si>
+    <t>08/06/2019</t>
+  </si>
+  <si>
+    <t>15/06/2019</t>
+  </si>
+  <si>
+    <t>Lastro</t>
   </si>
 </sst>
 </file>
@@ -671,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T51"/>
+  <dimension ref="A1:CG51"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -691,7 +699,7 @@
         <v>43617</v>
       </c>
       <c r="C1" s="8">
-        <v>43646</v>
+        <v>43676</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="18" customFormat="1" ht="15.75">
@@ -955,7 +963,7 @@
       <c r="S16" s="19"/>
       <c r="T16" s="19"/>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:85">
       <c r="A17" s="14" t="s">
         <v>8</v>
       </c>
@@ -979,7 +987,7 @@
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:85">
       <c r="A18" s="14" t="s">
         <v>9</v>
       </c>
@@ -1003,7 +1011,7 @@
       <c r="S18" s="19"/>
       <c r="T18" s="19"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:85">
       <c r="A19" s="14" t="s">
         <v>10</v>
       </c>
@@ -1027,31 +1035,261 @@
       <c r="S19" s="19"/>
       <c r="T19" s="19"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:85">
       <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19"/>
-      <c r="O20" s="19"/>
-      <c r="P20" s="19"/>
-      <c r="Q20" s="19"/>
-      <c r="R20" s="19"/>
-      <c r="S20" s="19"/>
-      <c r="T20" s="19"/>
-    </row>
-    <row r="21" spans="1:20">
+      <c r="B20" s="19">
+        <v>43647</v>
+      </c>
+      <c r="C20" s="19">
+        <v>43648</v>
+      </c>
+      <c r="D20" s="19">
+        <v>43649</v>
+      </c>
+      <c r="E20" s="19">
+        <v>43650</v>
+      </c>
+      <c r="F20" s="19">
+        <v>43651</v>
+      </c>
+      <c r="G20" s="19">
+        <v>43652</v>
+      </c>
+      <c r="H20" s="19">
+        <v>43653</v>
+      </c>
+      <c r="I20" s="19">
+        <v>43654</v>
+      </c>
+      <c r="J20" s="19">
+        <v>43655</v>
+      </c>
+      <c r="K20" s="19">
+        <v>43656</v>
+      </c>
+      <c r="L20" s="19">
+        <v>43657</v>
+      </c>
+      <c r="M20" s="19">
+        <v>43658</v>
+      </c>
+      <c r="N20" s="19">
+        <v>43659</v>
+      </c>
+      <c r="O20" s="19">
+        <v>43660</v>
+      </c>
+      <c r="P20" s="19">
+        <v>43661</v>
+      </c>
+      <c r="Q20" s="19">
+        <v>43662</v>
+      </c>
+      <c r="R20" s="19">
+        <v>43663</v>
+      </c>
+      <c r="S20" s="19">
+        <v>43664</v>
+      </c>
+      <c r="T20" s="19">
+        <v>43665</v>
+      </c>
+      <c r="U20" s="19">
+        <v>43666</v>
+      </c>
+      <c r="V20" s="19">
+        <v>43667</v>
+      </c>
+      <c r="W20" s="19">
+        <v>43668</v>
+      </c>
+      <c r="X20" s="19">
+        <v>43669</v>
+      </c>
+      <c r="Y20" s="19">
+        <v>43670</v>
+      </c>
+      <c r="Z20" s="19">
+        <v>43671</v>
+      </c>
+      <c r="AA20" s="19">
+        <v>43672</v>
+      </c>
+      <c r="AB20" s="19">
+        <v>43673</v>
+      </c>
+      <c r="AC20" s="19">
+        <v>43674</v>
+      </c>
+      <c r="AD20" s="19">
+        <v>43675</v>
+      </c>
+      <c r="AE20" s="19">
+        <v>43676</v>
+      </c>
+      <c r="AF20" s="19">
+        <v>43677</v>
+      </c>
+      <c r="AG20" s="19">
+        <v>43678</v>
+      </c>
+      <c r="AH20" s="19">
+        <v>43679</v>
+      </c>
+      <c r="AI20" s="19">
+        <v>43680</v>
+      </c>
+      <c r="AJ20" s="19">
+        <v>43681</v>
+      </c>
+      <c r="AK20" s="19">
+        <v>43682</v>
+      </c>
+      <c r="AL20" s="19">
+        <v>43683</v>
+      </c>
+      <c r="AM20" s="19">
+        <v>43684</v>
+      </c>
+      <c r="AN20" s="19">
+        <v>43685</v>
+      </c>
+      <c r="AO20" s="19">
+        <v>43686</v>
+      </c>
+      <c r="AP20" s="19">
+        <v>43687</v>
+      </c>
+      <c r="AQ20" s="19">
+        <v>43688</v>
+      </c>
+      <c r="AR20" s="19">
+        <v>43689</v>
+      </c>
+      <c r="AS20" s="19">
+        <v>43690</v>
+      </c>
+      <c r="AT20" s="19">
+        <v>43691</v>
+      </c>
+      <c r="AU20" s="19">
+        <v>43692</v>
+      </c>
+      <c r="AV20" s="19">
+        <v>43693</v>
+      </c>
+      <c r="AW20" s="19">
+        <v>43694</v>
+      </c>
+      <c r="AX20" s="19">
+        <v>43695</v>
+      </c>
+      <c r="AY20" s="19">
+        <v>43696</v>
+      </c>
+      <c r="AZ20" s="19">
+        <v>43697</v>
+      </c>
+      <c r="BA20" s="19">
+        <v>43698</v>
+      </c>
+      <c r="BB20" s="19">
+        <v>43699</v>
+      </c>
+      <c r="BC20" s="19">
+        <v>43700</v>
+      </c>
+      <c r="BD20" s="19">
+        <v>43701</v>
+      </c>
+      <c r="BE20" s="19">
+        <v>43702</v>
+      </c>
+      <c r="BF20" s="19">
+        <v>43703</v>
+      </c>
+      <c r="BG20" s="19">
+        <v>43704</v>
+      </c>
+      <c r="BH20" s="19">
+        <v>43705</v>
+      </c>
+      <c r="BI20" s="19">
+        <v>43706</v>
+      </c>
+      <c r="BJ20" s="19">
+        <v>43707</v>
+      </c>
+      <c r="BK20" s="19">
+        <v>43708</v>
+      </c>
+      <c r="BL20" s="19">
+        <v>43709</v>
+      </c>
+      <c r="BM20" s="19">
+        <v>43710</v>
+      </c>
+      <c r="BN20" s="19">
+        <v>43711</v>
+      </c>
+      <c r="BO20" s="19">
+        <v>43712</v>
+      </c>
+      <c r="BP20" s="19">
+        <v>43713</v>
+      </c>
+      <c r="BQ20" s="19">
+        <v>43714</v>
+      </c>
+      <c r="BR20" s="19">
+        <v>43715</v>
+      </c>
+      <c r="BS20" s="19">
+        <v>43716</v>
+      </c>
+      <c r="BT20" s="19">
+        <v>43717</v>
+      </c>
+      <c r="BU20" s="19">
+        <v>43718</v>
+      </c>
+      <c r="BV20" s="19">
+        <v>43719</v>
+      </c>
+      <c r="BW20" s="19">
+        <v>43720</v>
+      </c>
+      <c r="BX20" s="19">
+        <v>43721</v>
+      </c>
+      <c r="BY20" s="19">
+        <v>43722</v>
+      </c>
+      <c r="BZ20" s="19">
+        <v>43723</v>
+      </c>
+      <c r="CA20" s="19">
+        <v>43724</v>
+      </c>
+      <c r="CB20" s="19">
+        <v>43725</v>
+      </c>
+      <c r="CC20" s="19">
+        <v>43726</v>
+      </c>
+      <c r="CD20" s="19">
+        <v>43727</v>
+      </c>
+      <c r="CE20" s="19">
+        <v>43728</v>
+      </c>
+      <c r="CF20" s="19">
+        <v>43729</v>
+      </c>
+    </row>
+    <row r="21" spans="1:85">
       <c r="A21" s="14" t="s">
         <v>12</v>
       </c>
@@ -1075,7 +1313,7 @@
       <c r="S21" s="19"/>
       <c r="T21" s="19"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:85">
       <c r="A22" s="14" t="s">
         <v>13</v>
       </c>
@@ -1099,7 +1337,7 @@
       <c r="S22" s="19"/>
       <c r="T22" s="19"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:85">
       <c r="A23" s="14" t="s">
         <v>14</v>
       </c>
@@ -1123,7 +1361,7 @@
       <c r="S23" s="19"/>
       <c r="T23" s="19"/>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:85">
       <c r="A24" s="14" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1385,7 @@
       <c r="S24" s="19"/>
       <c r="T24" s="19"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:85">
       <c r="A25" s="14" t="s">
         <v>16</v>
       </c>
@@ -1171,7 +1409,7 @@
       <c r="S25" s="19"/>
       <c r="T25" s="19"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:85">
       <c r="A26" s="14" t="s">
         <v>17</v>
       </c>
@@ -1195,31 +1433,264 @@
       <c r="S26" s="19"/>
       <c r="T26" s="19"/>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:85">
       <c r="A27" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="19"/>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-      <c r="N27" s="19"/>
-      <c r="O27" s="19"/>
-      <c r="P27" s="19"/>
-      <c r="Q27" s="19"/>
-      <c r="R27" s="19"/>
-      <c r="S27" s="19"/>
-      <c r="T27" s="19"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="B27" s="19">
+        <v>43617</v>
+      </c>
+      <c r="C27" s="19">
+        <v>43618</v>
+      </c>
+      <c r="D27" s="19">
+        <v>43619</v>
+      </c>
+      <c r="E27" s="19">
+        <v>43620</v>
+      </c>
+      <c r="F27" s="19">
+        <v>43621</v>
+      </c>
+      <c r="G27" s="19">
+        <v>43622</v>
+      </c>
+      <c r="H27" s="19">
+        <v>43623</v>
+      </c>
+      <c r="I27" s="19">
+        <v>43624</v>
+      </c>
+      <c r="J27" s="19">
+        <v>43625</v>
+      </c>
+      <c r="K27" s="19">
+        <v>43626</v>
+      </c>
+      <c r="L27" s="19">
+        <v>43627</v>
+      </c>
+      <c r="M27" s="19">
+        <v>43628</v>
+      </c>
+      <c r="N27" s="19">
+        <v>43629</v>
+      </c>
+      <c r="O27" s="19">
+        <v>43630</v>
+      </c>
+      <c r="P27" s="19">
+        <v>43631</v>
+      </c>
+      <c r="Q27" s="19">
+        <v>43632</v>
+      </c>
+      <c r="R27" s="19">
+        <v>43633</v>
+      </c>
+      <c r="S27" s="19">
+        <v>43634</v>
+      </c>
+      <c r="T27" s="19">
+        <v>43635</v>
+      </c>
+      <c r="U27" s="19">
+        <v>43636</v>
+      </c>
+      <c r="V27" s="19">
+        <v>43637</v>
+      </c>
+      <c r="W27" s="19">
+        <v>43638</v>
+      </c>
+      <c r="X27" s="19">
+        <v>43639</v>
+      </c>
+      <c r="Y27" s="19">
+        <v>43640</v>
+      </c>
+      <c r="Z27" s="19">
+        <v>43641</v>
+      </c>
+      <c r="AA27" s="19">
+        <v>43642</v>
+      </c>
+      <c r="AB27" s="19">
+        <v>43643</v>
+      </c>
+      <c r="AC27" s="19">
+        <v>43644</v>
+      </c>
+      <c r="AD27" s="19">
+        <v>43645</v>
+      </c>
+      <c r="AE27" s="19">
+        <v>43646</v>
+      </c>
+      <c r="AF27" s="19">
+        <v>43647</v>
+      </c>
+      <c r="AG27" s="19">
+        <v>43648</v>
+      </c>
+      <c r="AH27" s="19">
+        <v>43649</v>
+      </c>
+      <c r="AI27" s="19">
+        <v>43650</v>
+      </c>
+      <c r="AJ27" s="19">
+        <v>43651</v>
+      </c>
+      <c r="AK27" s="19">
+        <v>43652</v>
+      </c>
+      <c r="AL27" s="19">
+        <v>43653</v>
+      </c>
+      <c r="AM27" s="19">
+        <v>43654</v>
+      </c>
+      <c r="AN27" s="19">
+        <v>43655</v>
+      </c>
+      <c r="AO27" s="19">
+        <v>43656</v>
+      </c>
+      <c r="AP27" s="19">
+        <v>43657</v>
+      </c>
+      <c r="AQ27" s="19">
+        <v>43658</v>
+      </c>
+      <c r="AR27" s="19">
+        <v>43659</v>
+      </c>
+      <c r="AS27" s="19">
+        <v>43660</v>
+      </c>
+      <c r="AT27" s="19">
+        <v>43661</v>
+      </c>
+      <c r="AU27" s="19">
+        <v>43662</v>
+      </c>
+      <c r="AV27" s="19">
+        <v>43663</v>
+      </c>
+      <c r="AW27" s="19">
+        <v>43664</v>
+      </c>
+      <c r="AX27" s="19">
+        <v>43665</v>
+      </c>
+      <c r="AY27" s="19">
+        <v>43666</v>
+      </c>
+      <c r="AZ27" s="19">
+        <v>43667</v>
+      </c>
+      <c r="BA27" s="19">
+        <v>43668</v>
+      </c>
+      <c r="BB27" s="19">
+        <v>43669</v>
+      </c>
+      <c r="BC27" s="19">
+        <v>43670</v>
+      </c>
+      <c r="BD27" s="19">
+        <v>43671</v>
+      </c>
+      <c r="BE27" s="19">
+        <v>43672</v>
+      </c>
+      <c r="BF27" s="19">
+        <v>43673</v>
+      </c>
+      <c r="BG27" s="19">
+        <v>43674</v>
+      </c>
+      <c r="BH27" s="19">
+        <v>43675</v>
+      </c>
+      <c r="BI27" s="19">
+        <v>43676</v>
+      </c>
+      <c r="BJ27" s="19">
+        <v>43677</v>
+      </c>
+      <c r="BK27" s="19">
+        <v>43678</v>
+      </c>
+      <c r="BL27" s="19">
+        <v>43679</v>
+      </c>
+      <c r="BM27" s="19">
+        <v>43680</v>
+      </c>
+      <c r="BN27" s="19">
+        <v>43681</v>
+      </c>
+      <c r="BO27" s="19">
+        <v>43682</v>
+      </c>
+      <c r="BP27" s="19">
+        <v>43683</v>
+      </c>
+      <c r="BQ27" s="19">
+        <v>43684</v>
+      </c>
+      <c r="BR27" s="19">
+        <v>43685</v>
+      </c>
+      <c r="BS27" s="19">
+        <v>43686</v>
+      </c>
+      <c r="BT27" s="19">
+        <v>43687</v>
+      </c>
+      <c r="BU27" s="19">
+        <v>43688</v>
+      </c>
+      <c r="BV27" s="19">
+        <v>43689</v>
+      </c>
+      <c r="BW27" s="19">
+        <v>43690</v>
+      </c>
+      <c r="BX27" s="19">
+        <v>43691</v>
+      </c>
+      <c r="BY27" s="19">
+        <v>43692</v>
+      </c>
+      <c r="BZ27" s="19">
+        <v>43693</v>
+      </c>
+      <c r="CA27" s="19">
+        <v>43694</v>
+      </c>
+      <c r="CB27" s="19">
+        <v>43695</v>
+      </c>
+      <c r="CC27" s="19">
+        <v>43696</v>
+      </c>
+      <c r="CD27" s="19">
+        <v>43697</v>
+      </c>
+      <c r="CE27" s="19">
+        <v>43698</v>
+      </c>
+      <c r="CF27" s="19">
+        <v>43699</v>
+      </c>
+      <c r="CG27" s="19">
+        <v>43700</v>
+      </c>
+    </row>
+    <row r="28" spans="1:85">
       <c r="A28" s="14" t="s">
         <v>19</v>
       </c>
@@ -1243,7 +1714,7 @@
       <c r="S28" s="19"/>
       <c r="T28" s="19"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:85">
       <c r="A29" s="14" t="s">
         <v>20</v>
       </c>
@@ -1267,7 +1738,7 @@
       <c r="S29" s="19"/>
       <c r="T29" s="19"/>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:85">
       <c r="A30" s="14" t="s">
         <v>21</v>
       </c>
@@ -1291,7 +1762,7 @@
       <c r="S30" s="19"/>
       <c r="T30" s="19"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:85">
       <c r="A31" s="14" t="s">
         <v>22</v>
       </c>
@@ -1315,7 +1786,7 @@
       <c r="S31" s="19"/>
       <c r="T31" s="19"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:85">
       <c r="A32" s="14" t="s">
         <v>23</v>
       </c>
@@ -1343,7 +1814,7 @@
       <c r="S32" s="19"/>
       <c r="T32" s="19"/>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:34">
       <c r="A33" s="14" t="s">
         <v>24</v>
       </c>
@@ -1369,7 +1840,7 @@
       <c r="S33" s="19"/>
       <c r="T33" s="19"/>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:34">
       <c r="A34" s="14" t="s">
         <v>25</v>
       </c>
@@ -1393,7 +1864,7 @@
       <c r="S34" s="19"/>
       <c r="T34" s="19"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:34">
       <c r="A35" s="14" t="s">
         <v>26</v>
       </c>
@@ -1419,31 +1890,111 @@
       <c r="S35" s="19"/>
       <c r="T35" s="19"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:34">
       <c r="A36" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="B36" s="19">
+        <v>43617</v>
+      </c>
+      <c r="C36" s="19">
+        <v>43618</v>
+      </c>
+      <c r="D36" s="19">
+        <v>43619</v>
+      </c>
+      <c r="E36" s="19">
+        <v>43620</v>
+      </c>
+      <c r="F36" s="19">
+        <v>43621</v>
+      </c>
+      <c r="G36" s="19">
+        <v>43622</v>
+      </c>
+      <c r="H36" s="19">
+        <v>43623</v>
+      </c>
+      <c r="I36" s="19">
+        <v>43624</v>
+      </c>
+      <c r="J36" s="19">
+        <v>43625</v>
+      </c>
+      <c r="K36" s="19">
+        <v>43626</v>
+      </c>
+      <c r="L36" s="19">
+        <v>43627</v>
+      </c>
+      <c r="M36" s="19">
+        <v>43628</v>
+      </c>
+      <c r="N36" s="19">
+        <v>43629</v>
+      </c>
+      <c r="O36" s="19">
+        <v>43630</v>
+      </c>
+      <c r="P36" s="19">
+        <v>43631</v>
+      </c>
+      <c r="Q36" s="19">
+        <v>43632</v>
+      </c>
+      <c r="R36" s="19">
+        <v>43633</v>
+      </c>
+      <c r="S36" s="19">
+        <v>43634</v>
+      </c>
+      <c r="T36" s="19">
+        <v>43635</v>
+      </c>
+      <c r="U36" s="19">
+        <v>43636</v>
+      </c>
+      <c r="V36" s="19">
+        <v>43637</v>
+      </c>
+      <c r="W36" s="19">
+        <v>43638</v>
+      </c>
+      <c r="X36" s="19">
+        <v>43639</v>
+      </c>
+      <c r="Y36" s="19">
+        <v>43640</v>
+      </c>
+      <c r="Z36" s="19">
+        <v>43641</v>
+      </c>
+      <c r="AA36" s="19">
+        <v>43642</v>
+      </c>
+      <c r="AB36" s="19">
+        <v>43643</v>
+      </c>
+      <c r="AC36" s="19">
+        <v>43644</v>
+      </c>
+      <c r="AD36" s="19">
+        <v>43645</v>
+      </c>
+      <c r="AE36" s="19">
+        <v>43646</v>
+      </c>
+      <c r="AF36" s="19">
+        <v>43647</v>
+      </c>
+      <c r="AG36" s="19">
+        <v>43648</v>
+      </c>
+      <c r="AH36" s="19">
+        <v>43649</v>
+      </c>
+    </row>
+    <row r="37" spans="1:34">
       <c r="A37" s="14" t="s">
         <v>28</v>
       </c>
@@ -1467,7 +2018,7 @@
       <c r="S37" s="19"/>
       <c r="T37" s="19"/>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:34">
       <c r="A38" s="14" t="s">
         <v>29</v>
       </c>
@@ -1493,7 +2044,7 @@
       <c r="S38" s="19"/>
       <c r="T38" s="19"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:34">
       <c r="A39" s="14" t="s">
         <v>30</v>
       </c>
@@ -1517,7 +2068,7 @@
       <c r="S39" s="19"/>
       <c r="T39" s="19"/>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:34">
       <c r="A40" s="14" t="s">
         <v>31</v>
       </c>
@@ -1541,7 +2092,7 @@
       <c r="S40" s="19"/>
       <c r="T40" s="19"/>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:34">
       <c r="A41" s="14" t="s">
         <v>32</v>
       </c>
@@ -1565,31 +2116,111 @@
       <c r="S41" s="19"/>
       <c r="T41" s="19"/>
     </row>
-    <row r="42" spans="1:20">
+    <row r="42" spans="1:34">
       <c r="A42" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
-      <c r="L42" s="19"/>
-      <c r="M42" s="19"/>
-      <c r="N42" s="19"/>
-      <c r="O42" s="19"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="19"/>
-      <c r="R42" s="19"/>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="B42" s="19">
+        <v>43617</v>
+      </c>
+      <c r="C42" s="19">
+        <v>43618</v>
+      </c>
+      <c r="D42" s="19">
+        <v>43619</v>
+      </c>
+      <c r="E42" s="19">
+        <v>43620</v>
+      </c>
+      <c r="F42" s="19">
+        <v>43621</v>
+      </c>
+      <c r="G42" s="19">
+        <v>43622</v>
+      </c>
+      <c r="H42" s="19">
+        <v>43623</v>
+      </c>
+      <c r="I42" s="19">
+        <v>43624</v>
+      </c>
+      <c r="J42" s="19">
+        <v>43625</v>
+      </c>
+      <c r="K42" s="19">
+        <v>43626</v>
+      </c>
+      <c r="L42" s="19">
+        <v>43627</v>
+      </c>
+      <c r="M42" s="19">
+        <v>43628</v>
+      </c>
+      <c r="N42" s="19">
+        <v>43629</v>
+      </c>
+      <c r="O42" s="19">
+        <v>43630</v>
+      </c>
+      <c r="P42" s="19">
+        <v>43631</v>
+      </c>
+      <c r="Q42" s="19">
+        <v>43632</v>
+      </c>
+      <c r="R42" s="19">
+        <v>43633</v>
+      </c>
+      <c r="S42" s="19">
+        <v>43634</v>
+      </c>
+      <c r="T42" s="19">
+        <v>43635</v>
+      </c>
+      <c r="U42" s="19">
+        <v>43636</v>
+      </c>
+      <c r="V42" s="19">
+        <v>43637</v>
+      </c>
+      <c r="W42" s="19">
+        <v>43638</v>
+      </c>
+      <c r="X42" s="19">
+        <v>43639</v>
+      </c>
+      <c r="Y42" s="19">
+        <v>43640</v>
+      </c>
+      <c r="Z42" s="19">
+        <v>43641</v>
+      </c>
+      <c r="AA42" s="19">
+        <v>43642</v>
+      </c>
+      <c r="AB42" s="19">
+        <v>43643</v>
+      </c>
+      <c r="AC42" s="19">
+        <v>43644</v>
+      </c>
+      <c r="AD42" s="19">
+        <v>43645</v>
+      </c>
+      <c r="AE42" s="19">
+        <v>43646</v>
+      </c>
+      <c r="AF42" s="19">
+        <v>43647</v>
+      </c>
+      <c r="AG42" s="19">
+        <v>43648</v>
+      </c>
+      <c r="AH42" s="19">
+        <v>43649</v>
+      </c>
+    </row>
+    <row r="43" spans="1:34">
       <c r="B43" s="19"/>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
@@ -1610,7 +2241,7 @@
       <c r="S43" s="19"/>
       <c r="T43" s="19"/>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:34">
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
       <c r="D44" s="19"/>
@@ -1631,7 +2262,7 @@
       <c r="S44" s="19"/>
       <c r="T44" s="19"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:34">
       <c r="B45" s="19"/>
       <c r="C45" s="19"/>
       <c r="D45" s="19"/>
@@ -1652,7 +2283,7 @@
       <c r="S45" s="19"/>
       <c r="T45" s="19"/>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:34">
       <c r="B46" s="19"/>
       <c r="C46" s="19"/>
       <c r="D46" s="19"/>
@@ -1673,7 +2304,7 @@
       <c r="S46" s="19"/>
       <c r="T46" s="19"/>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:34">
       <c r="B47" s="19"/>
       <c r="C47" s="19"/>
       <c r="D47" s="19"/>
@@ -1694,7 +2325,7 @@
       <c r="S47" s="19"/>
       <c r="T47" s="19"/>
     </row>
-    <row r="48" spans="1:20">
+    <row r="48" spans="1:34">
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
@@ -1789,11 +2420,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1835,212 +2464,209 @@
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:29" s="6" customFormat="1">
-      <c r="A2" s="27"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
+    <row r="2" spans="1:29">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="5" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>16</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1">
+        <v>43608</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1">
+        <v>43607</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1">
+        <v>43615</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43614</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43601</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="1">
-        <v>43631</v>
+        <v>30</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="4" t="s">
+      <c r="A36" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2051,10 +2677,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2070,181 +2696,181 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43454</v>
+      </c>
+    </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43454</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="4" t="s">
+      <c r="A36" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2255,10 +2881,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2274,178 +2900,178 @@
         <v>44</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="1:1">
       <c r="A3" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="5" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="4" t="s">
+      <c r="A36" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2456,10 +3082,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC37"/>
+  <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2503,200 +3129,191 @@
       <c r="AB1" s="26"/>
       <c r="AC1" s="26"/>
     </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" spans="1:29">
       <c r="A3" s="5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="5" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43641</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B33" s="1">
-        <v>43641</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43642</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B35" s="1">
-        <v>43642</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:2">
-      <c r="A36" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="4" t="s">
+      <c r="A36" s="4" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Tudo Ok (Falta organizar as posições da escala reserva)
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="46">
   <si>
     <t>1S SGS ANDERSON</t>
   </si>
@@ -153,12 +153,6 @@
   </si>
   <si>
     <t>MARROM</t>
-  </si>
-  <si>
-    <t>08/06/2019</t>
-  </si>
-  <si>
-    <t>15/06/2019</t>
   </si>
   <si>
     <t>Lastro</t>
@@ -679,10 +673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Plan1"/>
   <dimension ref="A1:CG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -2420,9 +2415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Plan2"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2553,11 +2549,11 @@
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>46</v>
+      <c r="B19" s="1">
+        <v>43624</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43631</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2639,30 +2635,29 @@
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="6"/>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>47</v>
+      <c r="B33" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>47</v>
+      <c r="B34" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>47</v>
+      <c r="B35" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2677,6 +2672,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Plan3"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -2881,6 +2877,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Plan4"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -3082,6 +3079,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Plan5"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -3204,7 +3202,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2">

</xml_diff>

<commit_message>
Inserito tipo de font no título
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -914,7 +914,7 @@
   <dimension ref="A1:CG51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="F4:H4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15"/>
@@ -929,10 +929,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="6">
-        <v>43678</v>
+        <v>43739</v>
       </c>
       <c r="C1" s="6">
-        <v>43708</v>
+        <v>43769</v>
       </c>
       <c r="E1" s="29" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
Corrigido Reserva da marrom e preta quem tem * no nome
</commit_message>
<xml_diff>
--- a/Escala.xlsx
+++ b/Escala.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="18735" windowHeight="8265" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Inicio" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="97">
   <si>
     <t>PERÍODO:</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>São José dos Campos, 9 de agosto de 2019</t>
+  </si>
+  <si>
+    <t>* Fora da escala Marrom</t>
+  </si>
+  <si>
+    <t>* Fora da escala Preta</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -654,6 +660,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,8 +958,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:CG51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -2236,9 +2243,7 @@
   <sheetPr codeName="Plan2"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:C34"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
@@ -2583,9 +2588,7 @@
   <sheetPr codeName="Plan3"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
@@ -2595,12 +2598,15 @@
     <col min="31" max="16384" width="10.7109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1">
       <c r="A1" s="24" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="F1" s="48" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="33" t="s">
         <v>8</v>
       </c>
@@ -2611,7 +2617,7 @@
         <v>43796</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" s="33" t="s">
         <v>9</v>
       </c>
@@ -2622,7 +2628,7 @@
         <v>43795</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4" s="33" t="s">
         <v>10</v>
       </c>
@@ -2633,7 +2639,7 @@
         <v>43794</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:6">
       <c r="A5" s="33" t="s">
         <v>11</v>
       </c>
@@ -2644,7 +2650,7 @@
         <v>43790</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:6">
       <c r="A6" s="33" t="s">
         <v>12</v>
       </c>
@@ -2655,7 +2661,7 @@
         <v>43789</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:6">
       <c r="A7" s="33" t="s">
         <v>13</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>43788</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:6">
       <c r="A8" s="33" t="s">
         <v>14</v>
       </c>
@@ -2677,7 +2683,7 @@
         <v>43787</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:6">
       <c r="A9" s="33" t="s">
         <v>44</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:6">
       <c r="A10" s="33" t="s">
         <v>16</v>
       </c>
@@ -2699,7 +2705,7 @@
         <v>43782</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:6">
       <c r="A11" s="33" t="s">
         <v>17</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>43781</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:6">
       <c r="A12" s="33" t="s">
         <v>18</v>
       </c>
@@ -2721,7 +2727,7 @@
         <v>43780</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:6">
       <c r="A13" s="33" t="s">
         <v>19</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>43776</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:6">
       <c r="A14" s="33" t="s">
         <v>20</v>
       </c>
@@ -2743,7 +2749,7 @@
         <v>43775</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:6">
       <c r="A15" s="33" t="s">
         <v>21</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>43774</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:6">
       <c r="A16" s="33" t="s">
         <v>22</v>
       </c>
@@ -2866,11 +2872,9 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="33">
-        <v>43810</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B26" s="33"/>
       <c r="C26" s="33"/>
     </row>
     <row r="27" spans="1:3">
@@ -2952,7 +2956,7 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="33" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" s="33"/>
       <c r="C34" s="33"/>
@@ -2992,8 +2996,8 @@
   <sheetPr codeName="Plan4"/>
   <dimension ref="A1:AC36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -3004,82 +3008,85 @@
     <col min="31" max="16384" width="10.7109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="26.25" customHeight="1">
+    <row r="1" spans="1:6" ht="26.25" customHeight="1">
       <c r="A1" s="26" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:1">
+      <c r="F1" s="48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="33" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:6">
       <c r="A3" s="33" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:6">
       <c r="A4" s="33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:6">
       <c r="A5" s="33" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:6">
       <c r="A6" s="33" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:6">
       <c r="A7" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:6">
       <c r="A8" s="33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:6">
       <c r="A9" s="33" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:6">
       <c r="A10" s="33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:6">
       <c r="A11" s="33" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:6">
       <c r="A12" s="33" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:6">
       <c r="A13" s="33" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:6">
       <c r="A14" s="33" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:6">
       <c r="A15" s="33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:6">
       <c r="A16" s="33" t="s">
         <v>22</v>
       </c>
@@ -3149,7 +3156,7 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="33" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B26" s="33"/>
     </row>
@@ -3211,7 +3218,7 @@
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="33" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B34" s="33"/>
     </row>
@@ -3233,6 +3240,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>